<commit_message>
New error with email class to be Resolved, Added assigning to Batch feature
</commit_message>
<xml_diff>
--- a/OfficerDetails.xlsx
+++ b/OfficerDetails.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -65,25 +65,34 @@
     <t>Djanae</t>
   </si>
   <si>
+    <t>Patterson2</t>
+  </si>
+  <si>
     <t>dwalsh@test.com</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>Contact@test.com</t>
+    <t>Pattersons</t>
+  </si>
+  <si>
+    <t>Contact@test.cool</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>Jame</t>
-  </si>
-  <si>
-    <t>Atlas</t>
-  </si>
-  <si>
-    <t>jessaj@test.com</t>
+    <t>Jessa</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Atlast</t>
+  </si>
+  <si>
+    <t>jj@test.works</t>
   </si>
 </sst>
 </file>
@@ -193,47 +202,47 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>